<commit_message>
added descriptions to metryki.xlsx
</commit_message>
<xml_diff>
--- a/metryki.xlsx
+++ b/metryki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidbrzakala/Python_RIS_nowy/Python_RIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C11C2-0AF2-B444-97CB-13F055707935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A58E7C2-606F-F445-9361-A046F1C5A090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>Pattern</t>
   </si>
@@ -47,12 +47,45 @@
   <si>
     <t>CC Znormalizowane</t>
   </si>
+  <si>
+    <t>Skrót</t>
+  </si>
+  <si>
+    <t>Sum Square Difference</t>
+  </si>
+  <si>
+    <t>Cross - Correlation</t>
+  </si>
+  <si>
+    <t>Mean Square Error</t>
+  </si>
+  <si>
+    <t>Opis</t>
+  </si>
+  <si>
+    <t>Rozwinięcie</t>
+  </si>
+  <si>
+    <t>Im mniejsza wartość MSE, tym obrazy są bardziej podobne.</t>
+  </si>
+  <si>
+    <t>Mean Absolute Error</t>
+  </si>
+  <si>
+    <t>Ocenia, jaka jest przeciętna różnica absolutna między odpowiadającymi sobie komórkami danych.</t>
+  </si>
+  <si>
+    <t>Im mniejsza wartość SSD, tym większe podobieństwo obrazów. Wrażliwy na duże różnice w wartościach (podnoszone do kwadratu).</t>
+  </si>
+  <si>
+    <t>Miara podobieństwa między obrazami, uwzględniająca przesunięcie (lub dopasowanie) jednego względem drugiego. Im większa wartość tym bardziej dopasowane.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +98,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,11 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -409,15 +460,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="126.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +498,17 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -462,8 +530,17 @@
       <c r="G2">
         <v>4618.5797481937543</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -485,8 +562,17 @@
       <c r="G3">
         <v>4757.2603060001029</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -508,8 +594,17 @@
       <c r="G4">
         <v>4619.1852721848118</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -531,8 +626,17 @@
       <c r="G5">
         <v>4622.6994378473928</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -555,7 +659,7 @@
         <v>4696.8973423467651</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -578,7 +682,7 @@
         <v>4637.0044429124946</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -601,7 +705,7 @@
         <v>4643.5975163074872</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -624,7 +728,7 @@
         <v>4591.8373034135566</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -647,7 +751,7 @@
         <v>4760.3681473342567</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -670,7 +774,7 @@
         <v>4716.6135533078068</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -693,7 +797,7 @@
         <v>4645.0235114485977</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -716,7 +820,7 @@
         <v>4646.0685059953266</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -739,7 +843,7 @@
         <v>4669.4640903271511</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -762,7 +866,7 @@
         <v>4653.5137598651154</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2388,7 +2492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC675B-C02A-EA44-970E-7C58E476B8DE}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates with nominal metrics file
</commit_message>
<xml_diff>
--- a/metryki.xlsx
+++ b/metryki.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidbrzakala/Python_RIS_nowy/Python_RIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A58E7C2-606F-F445-9361-A046F1C5A090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E456734-89A3-8C4C-A81D-40DAC41878FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId1"/>
-    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId2"/>
-    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId3"/>
-    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId4"/>
-    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId5"/>
-    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId6"/>
+    <sheet name="Przypadek_idealny" sheetId="7" r:id="rId1"/>
+    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId2"/>
+    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId3"/>
+    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId4"/>
+    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId5"/>
+    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId6"/>
+    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
   <si>
     <t>Pattern</t>
   </si>
@@ -459,11 +460,720 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66418B98-A566-1241-8A7F-C0F4C167C805}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="126.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>9607126294.2763863</v>
+      </c>
+      <c r="G2">
+        <v>5276.1340691461583</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>9537078371.3914661</v>
+      </c>
+      <c r="G3">
+        <v>5251.9100268661396</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>9704967193.7886658</v>
+      </c>
+      <c r="G4">
+        <v>5308.7961694239802</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>9655891525.2495346</v>
+      </c>
+      <c r="G5">
+        <v>5291.4859472277149</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>9493180688.7898598</v>
+      </c>
+      <c r="G6">
+        <v>5243.6565160137106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>9508391068.4208641</v>
+      </c>
+      <c r="G7">
+        <v>5246.0045394441267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>9341253730.1831856</v>
+      </c>
+      <c r="G8">
+        <v>5191.5504412444143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>9308171782.690506</v>
+      </c>
+      <c r="G9">
+        <v>5202.2256621001252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>9708761142.989624</v>
+      </c>
+      <c r="G10">
+        <v>5304.2327583285196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>9631875498.8010292</v>
+      </c>
+      <c r="G11">
+        <v>5268.5634248686883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>9435064987.509409</v>
+      </c>
+      <c r="G12">
+        <v>5210.9746656120251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>9459449891.3005981</v>
+      </c>
+      <c r="G13">
+        <v>5220.3136188947292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>9474660075.6223602</v>
+      </c>
+      <c r="G14">
+        <v>5226.2520645193972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>9412365552.6067162</v>
+      </c>
+      <c r="G15">
+        <v>5205.4834851355899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>9390075622.0031052</v>
+      </c>
+      <c r="G16">
+        <v>5232.4967643419232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>9311995833.2055168</v>
+      </c>
+      <c r="G17">
+        <v>5185.6943767462699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>9246922578.4275494</v>
+      </c>
+      <c r="G18">
+        <v>5174.9807500982988</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>9622749855.0244923</v>
+      </c>
+      <c r="G19">
+        <v>5291.7073133219919</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>9537654980.4943905</v>
+      </c>
+      <c r="G20">
+        <v>5266.0777400080378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>9350827020.8372917</v>
+      </c>
+      <c r="G21">
+        <v>5204.4192387542071</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>9543680685.8393612</v>
+      </c>
+      <c r="G22">
+        <v>5247.9698237055063</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>9327255860.2523842</v>
+      </c>
+      <c r="G23">
+        <v>5193.0167709651842</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>9226484504.3392639</v>
+      </c>
+      <c r="G24">
+        <v>5160.5891535931523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>9507893480.7103882</v>
+      </c>
+      <c r="G25">
+        <v>5256.9630666262756</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>9359400377.6798515</v>
+      </c>
+      <c r="G26">
+        <v>5203.8795893225979</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>9182893492.4142342</v>
+      </c>
+      <c r="G27">
+        <v>5146.3367599380499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>9115839822.3403645</v>
+      </c>
+      <c r="G28">
+        <v>5126.7030433348427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1170,7 +1880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E4EEC-6CC6-6348-84B2-EA3FB1DE8836}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -1829,7 +2539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E704B58D-6420-1E42-86AD-D07BE8D3A93C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2488,7 +3198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC675B-C02A-EA44-970E-7C58E476B8DE}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3147,7 +3857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF6E03A-F98C-914A-BDEA-46D84952CD42}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3806,7 +4516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C67EE-3E6E-F147-B360-22D732872280}">
   <dimension ref="A1:G28"/>
   <sheetViews>

</xml_diff>

<commit_message>
metryki - worst and best cases
</commit_message>
<xml_diff>
--- a/metryki.xlsx
+++ b/metryki.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidbrzakala/Python_RIS_nowy/Python_RIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E456734-89A3-8C4C-A81D-40DAC41878FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D048ADC-EC91-7042-8386-9D8DE80851D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Przypadek_idealny" sheetId="7" r:id="rId1"/>
-    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId2"/>
-    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId3"/>
-    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId4"/>
-    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId5"/>
-    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId6"/>
-    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId7"/>
+    <sheet name="Przypadek_najgorszy" sheetId="8" r:id="rId2"/>
+    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId3"/>
+    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId4"/>
+    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId5"/>
+    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId6"/>
+    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId7"/>
+    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="22">
   <si>
     <t>Pattern</t>
   </si>
@@ -81,12 +82,24 @@
   <si>
     <t>Miara podobieństwa między obrazami, uwzględniająca przesunięcie (lub dopasowanie) jednego względem drugiego. Im większa wartość tym bardziej dopasowane.</t>
   </si>
+  <si>
+    <t>W tym przypadku moce w pliku1 to -30dBm a w pliku2 -80dBm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W tym przypadku moce odebrane na obu plikach są takie same. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutaj oba pliki miały takie same moce odebrane -30dBm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutaj oba pliki miały moce odebrane  -80 dBm </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +127,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Tekst podstawowy)"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -159,6 +178,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -461,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66418B98-A566-1241-8A7F-C0F4C167C805}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,6 +722,9 @@
       <c r="G8">
         <v>5191.5504412444143</v>
       </c>
+      <c r="L8" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -887,7 +910,7 @@
         <v>5232.4967643419232</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -910,7 +933,7 @@
         <v>5185.6943767462699</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -933,7 +956,7 @@
         <v>5174.9807500982988</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -956,7 +979,7 @@
         <v>5291.7073133219919</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -979,7 +1002,7 @@
         <v>5266.0777400080378</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1002,7 +1025,7 @@
         <v>5204.4192387542071</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1025,7 +1048,7 @@
         <v>5247.9698237055063</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1048,7 +1071,7 @@
         <v>5193.0167709651842</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1071,7 +1094,7 @@
         <v>5160.5891535931523</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1094,7 +1117,7 @@
         <v>5256.9630666262756</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1117,7 +1140,7 @@
         <v>5203.8795893225979</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1140,7 +1163,7 @@
         <v>5146.3367599380499</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1161,6 +1184,1300 @@
       </c>
       <c r="G28">
         <v>5126.7030433348427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>289170000</v>
+      </c>
+      <c r="G32">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>289170000</v>
+      </c>
+      <c r="G33">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>289170000</v>
+      </c>
+      <c r="G34">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>289170000</v>
+      </c>
+      <c r="G35">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>289170000</v>
+      </c>
+      <c r="G36">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>289170000</v>
+      </c>
+      <c r="G37">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>289170000</v>
+      </c>
+      <c r="G38">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>289170000</v>
+      </c>
+      <c r="G39">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>289170000</v>
+      </c>
+      <c r="G40">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>289170000</v>
+      </c>
+      <c r="G41">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>289170000</v>
+      </c>
+      <c r="G42">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>289170000</v>
+      </c>
+      <c r="G43">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>289170000</v>
+      </c>
+      <c r="G44">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>289170000</v>
+      </c>
+      <c r="G45">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>289170000</v>
+      </c>
+      <c r="G46">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>289170000</v>
+      </c>
+      <c r="G47">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>289170000</v>
+      </c>
+      <c r="G48">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>289170000</v>
+      </c>
+      <c r="G49">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>19</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>289170000</v>
+      </c>
+      <c r="G50">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>289170000</v>
+      </c>
+      <c r="G51">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>289170000</v>
+      </c>
+      <c r="G52">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>22</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>289170000</v>
+      </c>
+      <c r="G53">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>289170000</v>
+      </c>
+      <c r="G54">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>289170000</v>
+      </c>
+      <c r="G55">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>25</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>289170000</v>
+      </c>
+      <c r="G56">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>289170000</v>
+      </c>
+      <c r="G57">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>27</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>289170000</v>
+      </c>
+      <c r="G58">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>14622720000</v>
+      </c>
+      <c r="G62">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>14622720000</v>
+      </c>
+      <c r="G63">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>14622720000</v>
+      </c>
+      <c r="G64">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>14622720000</v>
+      </c>
+      <c r="G65">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>14622720000</v>
+      </c>
+      <c r="G66">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>14622720000</v>
+      </c>
+      <c r="G67">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>14622720000</v>
+      </c>
+      <c r="G68">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>14622720000</v>
+      </c>
+      <c r="G69">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>14622720000</v>
+      </c>
+      <c r="G70">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>14622720000</v>
+      </c>
+      <c r="G71">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>14622720000</v>
+      </c>
+      <c r="G72">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>12</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>14622720000</v>
+      </c>
+      <c r="G73">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>14622720000</v>
+      </c>
+      <c r="G74">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>14</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>14622720000</v>
+      </c>
+      <c r="G75">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>14622720000</v>
+      </c>
+      <c r="G76">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>16</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>14622720000</v>
+      </c>
+      <c r="G77">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>17</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>14622720000</v>
+      </c>
+      <c r="G78">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>14622720000</v>
+      </c>
+      <c r="G79">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>14622720000</v>
+      </c>
+      <c r="G80">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>20</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>14622720000</v>
+      </c>
+      <c r="G81">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>21</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>14622720000</v>
+      </c>
+      <c r="G82">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>22</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>14622720000</v>
+      </c>
+      <c r="G83">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>14622720000</v>
+      </c>
+      <c r="G84">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>24</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>14622720000</v>
+      </c>
+      <c r="G85">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>25</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>14622720000</v>
+      </c>
+      <c r="G86">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>26</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>14622720000</v>
+      </c>
+      <c r="G87">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>27</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>14622720000</v>
+      </c>
+      <c r="G88">
+        <v>6400</v>
       </c>
     </row>
   </sheetData>
@@ -1169,6 +2486,716 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CFAE75-F157-724D-A078-62EE8629F77D}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="126.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2500</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>892500</v>
+      </c>
+      <c r="E2">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F2">
+        <v>2056320000</v>
+      </c>
+      <c r="G2">
+        <v>2400</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2500</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>892500</v>
+      </c>
+      <c r="E3">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F3">
+        <v>2056320000</v>
+      </c>
+      <c r="G3">
+        <v>2400</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2500</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>892500</v>
+      </c>
+      <c r="E4">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F4">
+        <v>2056320000</v>
+      </c>
+      <c r="G4">
+        <v>2400</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2500</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>892500</v>
+      </c>
+      <c r="E5">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F5">
+        <v>2056320000</v>
+      </c>
+      <c r="G5">
+        <v>2400</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>892500</v>
+      </c>
+      <c r="E6">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F6">
+        <v>2056320000</v>
+      </c>
+      <c r="G6">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2500</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>892500</v>
+      </c>
+      <c r="E7">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F7">
+        <v>2056320000</v>
+      </c>
+      <c r="G7">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2500</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>892500</v>
+      </c>
+      <c r="E8">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F8">
+        <v>2056320000</v>
+      </c>
+      <c r="G8">
+        <v>2400</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2500</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>892500</v>
+      </c>
+      <c r="E9">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F9">
+        <v>2056320000</v>
+      </c>
+      <c r="G9">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2500</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>892500</v>
+      </c>
+      <c r="E10">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F10">
+        <v>2056320000</v>
+      </c>
+      <c r="G10">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2500</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>892500</v>
+      </c>
+      <c r="E11">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F11">
+        <v>2056320000</v>
+      </c>
+      <c r="G11">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2500</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>892500</v>
+      </c>
+      <c r="E12">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F12">
+        <v>2056320000</v>
+      </c>
+      <c r="G12">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2500</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>892500</v>
+      </c>
+      <c r="E13">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F13">
+        <v>2056320000</v>
+      </c>
+      <c r="G13">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2500</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>892500</v>
+      </c>
+      <c r="E14">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F14">
+        <v>2056320000</v>
+      </c>
+      <c r="G14">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2500</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>892500</v>
+      </c>
+      <c r="E15">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F15">
+        <v>2056320000</v>
+      </c>
+      <c r="G15">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2500</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>892500</v>
+      </c>
+      <c r="E16">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F16">
+        <v>2056320000</v>
+      </c>
+      <c r="G16">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2500</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>892500</v>
+      </c>
+      <c r="E17">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F17">
+        <v>2056320000</v>
+      </c>
+      <c r="G17">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2500</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>892500</v>
+      </c>
+      <c r="E18">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F18">
+        <v>2056320000</v>
+      </c>
+      <c r="G18">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2500</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <v>892500</v>
+      </c>
+      <c r="E19">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F19">
+        <v>2056320000</v>
+      </c>
+      <c r="G19">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2500</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="D20">
+        <v>892500</v>
+      </c>
+      <c r="E20">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F20">
+        <v>2056320000</v>
+      </c>
+      <c r="G20">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2500</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>892500</v>
+      </c>
+      <c r="E21">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F21">
+        <v>2056320000</v>
+      </c>
+      <c r="G21">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2500</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>892500</v>
+      </c>
+      <c r="E22">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F22">
+        <v>2056320000</v>
+      </c>
+      <c r="G22">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2500</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>892500</v>
+      </c>
+      <c r="E23">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F23">
+        <v>2056320000</v>
+      </c>
+      <c r="G23">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2500</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>892500</v>
+      </c>
+      <c r="E24">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F24">
+        <v>2056320000</v>
+      </c>
+      <c r="G24">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2500</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25">
+        <v>892500</v>
+      </c>
+      <c r="E25">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F25">
+        <v>2056320000</v>
+      </c>
+      <c r="G25">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2500</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26">
+        <v>892500</v>
+      </c>
+      <c r="E26">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F26">
+        <v>2056320000</v>
+      </c>
+      <c r="G26">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2500</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>892500</v>
+      </c>
+      <c r="E27">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F27">
+        <v>2056320000</v>
+      </c>
+      <c r="G27">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>2500</v>
+      </c>
+      <c r="C28">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>892500</v>
+      </c>
+      <c r="E28">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F28">
+        <v>2056320000</v>
+      </c>
+      <c r="G28">
+        <v>2400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
@@ -1880,7 +3907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E4EEC-6CC6-6348-84B2-EA3FB1DE8836}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2539,7 +4566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E704B58D-6420-1E42-86AD-D07BE8D3A93C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3198,7 +5225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC675B-C02A-EA44-970E-7C58E476B8DE}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3857,7 +5884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF6E03A-F98C-914A-BDEA-46D84952CD42}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -4516,7 +6543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C67EE-3E6E-F147-B360-22D732872280}">
   <dimension ref="A1:G28"/>
   <sheetViews>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/RISurfaces/Python_RIS"
This reverts commit 3d3083be379e944b150ce9c807576247d91b3316, reversing
changes made to 240f2135aad681a141113fd5fe944e75f053fc3e.
</commit_message>
<xml_diff>
--- a/metryki.xlsx
+++ b/metryki.xlsx
@@ -8,26 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidbrzakala/Python_RIS_nowy/Python_RIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D048ADC-EC91-7042-8386-9D8DE80851D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E456734-89A3-8C4C-A81D-40DAC41878FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Przypadek_idealny" sheetId="7" r:id="rId1"/>
-    <sheet name="Przypadek_najgorszy" sheetId="8" r:id="rId2"/>
-    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId3"/>
-    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId4"/>
-    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId5"/>
-    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId6"/>
-    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId7"/>
-    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId8"/>
+    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId2"/>
+    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId3"/>
+    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId4"/>
+    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId5"/>
+    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId6"/>
+    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
   <si>
     <t>Pattern</t>
   </si>
@@ -82,24 +81,12 @@
   <si>
     <t>Miara podobieństwa między obrazami, uwzględniająca przesunięcie (lub dopasowanie) jednego względem drugiego. Im większa wartość tym bardziej dopasowane.</t>
   </si>
-  <si>
-    <t>W tym przypadku moce w pliku1 to -30dBm a w pliku2 -80dBm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W tym przypadku moce odebrane na obu plikach są takie same. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutaj oba pliki miały takie same moce odebrane -30dBm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutaj oba pliki miały moce odebrane  -80 dBm </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,12 +114,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Tekst podstawowy)"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -178,7 +159,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -481,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66418B98-A566-1241-8A7F-C0F4C167C805}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -722,9 +702,6 @@
       <c r="G8">
         <v>5191.5504412444143</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -910,7 +887,7 @@
         <v>5232.4967643419232</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -933,7 +910,7 @@
         <v>5185.6943767462699</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -956,7 +933,7 @@
         <v>5174.9807500982988</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -979,7 +956,7 @@
         <v>5291.7073133219919</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1002,7 +979,7 @@
         <v>5266.0777400080378</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1025,7 +1002,7 @@
         <v>5204.4192387542071</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1048,7 +1025,7 @@
         <v>5247.9698237055063</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1071,7 +1048,7 @@
         <v>5193.0167709651842</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1094,7 +1071,7 @@
         <v>5160.5891535931523</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1117,7 +1094,7 @@
         <v>5256.9630666262756</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1140,7 +1117,7 @@
         <v>5203.8795893225979</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1163,7 +1140,7 @@
         <v>5146.3367599380499</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1184,1300 +1161,6 @@
       </c>
       <c r="G28">
         <v>5126.7030433348427</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>289170000</v>
-      </c>
-      <c r="G32">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>2</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>289170000</v>
-      </c>
-      <c r="G33">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>289170000</v>
-      </c>
-      <c r="G34">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>4</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>289170000</v>
-      </c>
-      <c r="G35">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>5</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>289170000</v>
-      </c>
-      <c r="G36">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>6</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>289170000</v>
-      </c>
-      <c r="G37">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>7</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>289170000</v>
-      </c>
-      <c r="G38">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>8</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>289170000</v>
-      </c>
-      <c r="G39">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>9</v>
-      </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>289170000</v>
-      </c>
-      <c r="G40">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>10</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>289170000</v>
-      </c>
-      <c r="G41">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>11</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>289170000</v>
-      </c>
-      <c r="G42">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>12</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>289170000</v>
-      </c>
-      <c r="G43">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>13</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>289170000</v>
-      </c>
-      <c r="G44">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>14</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>289170000</v>
-      </c>
-      <c r="G45">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>15</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>289170000</v>
-      </c>
-      <c r="G46">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>16</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>289170000</v>
-      </c>
-      <c r="G47">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>17</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>289170000</v>
-      </c>
-      <c r="G48">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>18</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>289170000</v>
-      </c>
-      <c r="G49">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>19</v>
-      </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>289170000</v>
-      </c>
-      <c r="G50">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>20</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>289170000</v>
-      </c>
-      <c r="G51">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>21</v>
-      </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>289170000</v>
-      </c>
-      <c r="G52">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>22</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>289170000</v>
-      </c>
-      <c r="G53">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>23</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>289170000</v>
-      </c>
-      <c r="G54">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>24</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>289170000</v>
-      </c>
-      <c r="G55">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>25</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>289170000</v>
-      </c>
-      <c r="G56">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>26</v>
-      </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>289170000</v>
-      </c>
-      <c r="G57">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>27</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>289170000</v>
-      </c>
-      <c r="G58">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L61" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>1</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>14622720000</v>
-      </c>
-      <c r="G62">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>2</v>
-      </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>14622720000</v>
-      </c>
-      <c r="G63">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>3</v>
-      </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
-        <v>14622720000</v>
-      </c>
-      <c r="G64">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>4</v>
-      </c>
-      <c r="B65">
-        <v>0</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>14622720000</v>
-      </c>
-      <c r="G65">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>5</v>
-      </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <v>14622720000</v>
-      </c>
-      <c r="G66">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>6</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>14622720000</v>
-      </c>
-      <c r="G67">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>7</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>14622720000</v>
-      </c>
-      <c r="G68">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>8</v>
-      </c>
-      <c r="B69">
-        <v>0</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>14622720000</v>
-      </c>
-      <c r="G69">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>9</v>
-      </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>14622720000</v>
-      </c>
-      <c r="G70">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>10</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>14622720000</v>
-      </c>
-      <c r="G71">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>11</v>
-      </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>14622720000</v>
-      </c>
-      <c r="G72">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>12</v>
-      </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73">
-        <v>14622720000</v>
-      </c>
-      <c r="G73">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>13</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>14622720000</v>
-      </c>
-      <c r="G74">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>14</v>
-      </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>14622720000</v>
-      </c>
-      <c r="G75">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>15</v>
-      </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>14622720000</v>
-      </c>
-      <c r="G76">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>16</v>
-      </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>14622720000</v>
-      </c>
-      <c r="G77">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>17</v>
-      </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>14622720000</v>
-      </c>
-      <c r="G78">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>18</v>
-      </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>14622720000</v>
-      </c>
-      <c r="G79">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>19</v>
-      </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>14622720000</v>
-      </c>
-      <c r="G80">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>20</v>
-      </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="F81">
-        <v>14622720000</v>
-      </c>
-      <c r="G81">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>21</v>
-      </c>
-      <c r="B82">
-        <v>0</v>
-      </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="F82">
-        <v>14622720000</v>
-      </c>
-      <c r="G82">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>22</v>
-      </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>14622720000</v>
-      </c>
-      <c r="G83">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>23</v>
-      </c>
-      <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>14622720000</v>
-      </c>
-      <c r="G84">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>24</v>
-      </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="F85">
-        <v>14622720000</v>
-      </c>
-      <c r="G85">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>25</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
-        <v>0</v>
-      </c>
-      <c r="F86">
-        <v>14622720000</v>
-      </c>
-      <c r="G86">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>26</v>
-      </c>
-      <c r="B87">
-        <v>0</v>
-      </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-      <c r="E87">
-        <v>0</v>
-      </c>
-      <c r="F87">
-        <v>14622720000</v>
-      </c>
-      <c r="G87">
-        <v>6400</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>27</v>
-      </c>
-      <c r="B88">
-        <v>0</v>
-      </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-      <c r="E88">
-        <v>0</v>
-      </c>
-      <c r="F88">
-        <v>14622720000</v>
-      </c>
-      <c r="G88">
-        <v>6400</v>
       </c>
     </row>
   </sheetData>
@@ -2486,716 +1169,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CFAE75-F157-724D-A078-62EE8629F77D}">
-  <dimension ref="A1:L28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="12" max="12" width="126.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2500</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>892500</v>
-      </c>
-      <c r="E2">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F2">
-        <v>2056320000</v>
-      </c>
-      <c r="G2">
-        <v>2400</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2500</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>892500</v>
-      </c>
-      <c r="E3">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F3">
-        <v>2056320000</v>
-      </c>
-      <c r="G3">
-        <v>2400</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2500</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>892500</v>
-      </c>
-      <c r="E4">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F4">
-        <v>2056320000</v>
-      </c>
-      <c r="G4">
-        <v>2400</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2500</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>892500</v>
-      </c>
-      <c r="E5">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F5">
-        <v>2056320000</v>
-      </c>
-      <c r="G5">
-        <v>2400</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2500</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>892500</v>
-      </c>
-      <c r="E6">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F6">
-        <v>2056320000</v>
-      </c>
-      <c r="G6">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2500</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7">
-        <v>892500</v>
-      </c>
-      <c r="E7">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F7">
-        <v>2056320000</v>
-      </c>
-      <c r="G7">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2500</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <v>892500</v>
-      </c>
-      <c r="E8">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F8">
-        <v>2056320000</v>
-      </c>
-      <c r="G8">
-        <v>2400</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2500</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <v>892500</v>
-      </c>
-      <c r="E9">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F9">
-        <v>2056320000</v>
-      </c>
-      <c r="G9">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>2500</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <v>892500</v>
-      </c>
-      <c r="E10">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F10">
-        <v>2056320000</v>
-      </c>
-      <c r="G10">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2500</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11">
-        <v>892500</v>
-      </c>
-      <c r="E11">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F11">
-        <v>2056320000</v>
-      </c>
-      <c r="G11">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>2500</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12">
-        <v>892500</v>
-      </c>
-      <c r="E12">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F12">
-        <v>2056320000</v>
-      </c>
-      <c r="G12">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2500</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13">
-        <v>892500</v>
-      </c>
-      <c r="E13">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F13">
-        <v>2056320000</v>
-      </c>
-      <c r="G13">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2500</v>
-      </c>
-      <c r="C14">
-        <v>50</v>
-      </c>
-      <c r="D14">
-        <v>892500</v>
-      </c>
-      <c r="E14">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F14">
-        <v>2056320000</v>
-      </c>
-      <c r="G14">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2500</v>
-      </c>
-      <c r="C15">
-        <v>50</v>
-      </c>
-      <c r="D15">
-        <v>892500</v>
-      </c>
-      <c r="E15">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F15">
-        <v>2056320000</v>
-      </c>
-      <c r="G15">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>2500</v>
-      </c>
-      <c r="C16">
-        <v>50</v>
-      </c>
-      <c r="D16">
-        <v>892500</v>
-      </c>
-      <c r="E16">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F16">
-        <v>2056320000</v>
-      </c>
-      <c r="G16">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>2500</v>
-      </c>
-      <c r="C17">
-        <v>50</v>
-      </c>
-      <c r="D17">
-        <v>892500</v>
-      </c>
-      <c r="E17">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F17">
-        <v>2056320000</v>
-      </c>
-      <c r="G17">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>2500</v>
-      </c>
-      <c r="C18">
-        <v>50</v>
-      </c>
-      <c r="D18">
-        <v>892500</v>
-      </c>
-      <c r="E18">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F18">
-        <v>2056320000</v>
-      </c>
-      <c r="G18">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>2500</v>
-      </c>
-      <c r="C19">
-        <v>50</v>
-      </c>
-      <c r="D19">
-        <v>892500</v>
-      </c>
-      <c r="E19">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F19">
-        <v>2056320000</v>
-      </c>
-      <c r="G19">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>2500</v>
-      </c>
-      <c r="C20">
-        <v>50</v>
-      </c>
-      <c r="D20">
-        <v>892500</v>
-      </c>
-      <c r="E20">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F20">
-        <v>2056320000</v>
-      </c>
-      <c r="G20">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>2500</v>
-      </c>
-      <c r="C21">
-        <v>50</v>
-      </c>
-      <c r="D21">
-        <v>892500</v>
-      </c>
-      <c r="E21">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F21">
-        <v>2056320000</v>
-      </c>
-      <c r="G21">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>2500</v>
-      </c>
-      <c r="C22">
-        <v>50</v>
-      </c>
-      <c r="D22">
-        <v>892500</v>
-      </c>
-      <c r="E22">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F22">
-        <v>2056320000</v>
-      </c>
-      <c r="G22">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>2500</v>
-      </c>
-      <c r="C23">
-        <v>50</v>
-      </c>
-      <c r="D23">
-        <v>892500</v>
-      </c>
-      <c r="E23">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F23">
-        <v>2056320000</v>
-      </c>
-      <c r="G23">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>2500</v>
-      </c>
-      <c r="C24">
-        <v>50</v>
-      </c>
-      <c r="D24">
-        <v>892500</v>
-      </c>
-      <c r="E24">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F24">
-        <v>2056320000</v>
-      </c>
-      <c r="G24">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>2500</v>
-      </c>
-      <c r="C25">
-        <v>50</v>
-      </c>
-      <c r="D25">
-        <v>892500</v>
-      </c>
-      <c r="E25">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F25">
-        <v>2056320000</v>
-      </c>
-      <c r="G25">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>2500</v>
-      </c>
-      <c r="C26">
-        <v>50</v>
-      </c>
-      <c r="D26">
-        <v>892500</v>
-      </c>
-      <c r="E26">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F26">
-        <v>2056320000</v>
-      </c>
-      <c r="G26">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>2500</v>
-      </c>
-      <c r="C27">
-        <v>50</v>
-      </c>
-      <c r="D27">
-        <v>892500</v>
-      </c>
-      <c r="E27">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F27">
-        <v>2056320000</v>
-      </c>
-      <c r="G27">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>2500</v>
-      </c>
-      <c r="C28">
-        <v>50</v>
-      </c>
-      <c r="D28">
-        <v>892500</v>
-      </c>
-      <c r="E28">
-        <v>1.041666666666667</v>
-      </c>
-      <c r="F28">
-        <v>2056320000</v>
-      </c>
-      <c r="G28">
-        <v>2400</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
@@ -3907,7 +1880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E4EEC-6CC6-6348-84B2-EA3FB1DE8836}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -4566,7 +2539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E704B58D-6420-1E42-86AD-D07BE8D3A93C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -5225,7 +3198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC675B-C02A-EA44-970E-7C58E476B8DE}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -5884,7 +3857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF6E03A-F98C-914A-BDEA-46D84952CD42}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -6543,7 +4516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C67EE-3E6E-F147-B360-22D732872280}">
   <dimension ref="A1:G28"/>
   <sheetViews>

</xml_diff>

<commit_message>
Reapply "Merge branch 'main' of https://github.com/RISurfaces/Python_RIS"
This reverts commit 6fef844ac9f130e2998016f3e30e66b30e895a54.
</commit_message>
<xml_diff>
--- a/metryki.xlsx
+++ b/metryki.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidbrzakala/Python_RIS_nowy/Python_RIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E456734-89A3-8C4C-A81D-40DAC41878FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D048ADC-EC91-7042-8386-9D8DE80851D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Przypadek_idealny" sheetId="7" r:id="rId1"/>
-    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId2"/>
-    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId3"/>
-    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId4"/>
-    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId5"/>
-    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId6"/>
-    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId7"/>
+    <sheet name="Przypadek_najgorszy" sheetId="8" r:id="rId2"/>
+    <sheet name="METIS_AINFO_1m" sheetId="1" r:id="rId3"/>
+    <sheet name="METIS_AINFO_1.5m" sheetId="2" r:id="rId4"/>
+    <sheet name="METIS_AINFO_2m" sheetId="3" r:id="rId5"/>
+    <sheet name="METIS_KOMORA_1m" sheetId="4" r:id="rId6"/>
+    <sheet name="METIS_KOMORA_1.5m" sheetId="5" r:id="rId7"/>
+    <sheet name="METIS_KOMORA_2m" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="22">
   <si>
     <t>Pattern</t>
   </si>
@@ -81,12 +82,24 @@
   <si>
     <t>Miara podobieństwa między obrazami, uwzględniająca przesunięcie (lub dopasowanie) jednego względem drugiego. Im większa wartość tym bardziej dopasowane.</t>
   </si>
+  <si>
+    <t>W tym przypadku moce w pliku1 to -30dBm a w pliku2 -80dBm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W tym przypadku moce odebrane na obu plikach są takie same. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutaj oba pliki miały takie same moce odebrane -30dBm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutaj oba pliki miały moce odebrane  -80 dBm </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +127,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Tekst podstawowy)"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -159,6 +178,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -461,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66418B98-A566-1241-8A7F-C0F4C167C805}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,6 +722,9 @@
       <c r="G8">
         <v>5191.5504412444143</v>
       </c>
+      <c r="L8" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -887,7 +910,7 @@
         <v>5232.4967643419232</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -910,7 +933,7 @@
         <v>5185.6943767462699</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -933,7 +956,7 @@
         <v>5174.9807500982988</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -956,7 +979,7 @@
         <v>5291.7073133219919</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -979,7 +1002,7 @@
         <v>5266.0777400080378</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1002,7 +1025,7 @@
         <v>5204.4192387542071</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1025,7 +1048,7 @@
         <v>5247.9698237055063</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1048,7 +1071,7 @@
         <v>5193.0167709651842</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1071,7 +1094,7 @@
         <v>5160.5891535931523</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1094,7 +1117,7 @@
         <v>5256.9630666262756</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1117,7 +1140,7 @@
         <v>5203.8795893225979</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1140,7 +1163,7 @@
         <v>5146.3367599380499</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1161,6 +1184,1300 @@
       </c>
       <c r="G28">
         <v>5126.7030433348427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>289170000</v>
+      </c>
+      <c r="G32">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>289170000</v>
+      </c>
+      <c r="G33">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>289170000</v>
+      </c>
+      <c r="G34">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>289170000</v>
+      </c>
+      <c r="G35">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>289170000</v>
+      </c>
+      <c r="G36">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>289170000</v>
+      </c>
+      <c r="G37">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>289170000</v>
+      </c>
+      <c r="G38">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>289170000</v>
+      </c>
+      <c r="G39">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>289170000</v>
+      </c>
+      <c r="G40">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>289170000</v>
+      </c>
+      <c r="G41">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>289170000</v>
+      </c>
+      <c r="G42">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>289170000</v>
+      </c>
+      <c r="G43">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>289170000</v>
+      </c>
+      <c r="G44">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>289170000</v>
+      </c>
+      <c r="G45">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>289170000</v>
+      </c>
+      <c r="G46">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>289170000</v>
+      </c>
+      <c r="G47">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>289170000</v>
+      </c>
+      <c r="G48">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>18</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>289170000</v>
+      </c>
+      <c r="G49">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>19</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>289170000</v>
+      </c>
+      <c r="G50">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>289170000</v>
+      </c>
+      <c r="G51">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>21</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>289170000</v>
+      </c>
+      <c r="G52">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>22</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>289170000</v>
+      </c>
+      <c r="G53">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>289170000</v>
+      </c>
+      <c r="G54">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>24</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>289170000</v>
+      </c>
+      <c r="G55">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>25</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>289170000</v>
+      </c>
+      <c r="G56">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>289170000</v>
+      </c>
+      <c r="G57">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>27</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>289170000</v>
+      </c>
+      <c r="G58">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>14622720000</v>
+      </c>
+      <c r="G62">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>14622720000</v>
+      </c>
+      <c r="G63">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>14622720000</v>
+      </c>
+      <c r="G64">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>14622720000</v>
+      </c>
+      <c r="G65">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>14622720000</v>
+      </c>
+      <c r="G66">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>14622720000</v>
+      </c>
+      <c r="G67">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>14622720000</v>
+      </c>
+      <c r="G68">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>14622720000</v>
+      </c>
+      <c r="G69">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>14622720000</v>
+      </c>
+      <c r="G70">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>14622720000</v>
+      </c>
+      <c r="G71">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>14622720000</v>
+      </c>
+      <c r="G72">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>12</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>14622720000</v>
+      </c>
+      <c r="G73">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>14622720000</v>
+      </c>
+      <c r="G74">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>14</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>14622720000</v>
+      </c>
+      <c r="G75">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>14622720000</v>
+      </c>
+      <c r="G76">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>16</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>14622720000</v>
+      </c>
+      <c r="G77">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>17</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>14622720000</v>
+      </c>
+      <c r="G78">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>14622720000</v>
+      </c>
+      <c r="G79">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>14622720000</v>
+      </c>
+      <c r="G80">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>20</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>14622720000</v>
+      </c>
+      <c r="G81">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>21</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>14622720000</v>
+      </c>
+      <c r="G82">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>22</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>14622720000</v>
+      </c>
+      <c r="G83">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>14622720000</v>
+      </c>
+      <c r="G84">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>24</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>14622720000</v>
+      </c>
+      <c r="G85">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>25</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>14622720000</v>
+      </c>
+      <c r="G86">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>26</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>14622720000</v>
+      </c>
+      <c r="G87">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>27</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>14622720000</v>
+      </c>
+      <c r="G88">
+        <v>6400</v>
       </c>
     </row>
   </sheetData>
@@ -1169,6 +2486,716 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CFAE75-F157-724D-A078-62EE8629F77D}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="126.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2500</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>892500</v>
+      </c>
+      <c r="E2">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F2">
+        <v>2056320000</v>
+      </c>
+      <c r="G2">
+        <v>2400</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2500</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>892500</v>
+      </c>
+      <c r="E3">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F3">
+        <v>2056320000</v>
+      </c>
+      <c r="G3">
+        <v>2400</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2500</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>892500</v>
+      </c>
+      <c r="E4">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F4">
+        <v>2056320000</v>
+      </c>
+      <c r="G4">
+        <v>2400</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2500</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>892500</v>
+      </c>
+      <c r="E5">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F5">
+        <v>2056320000</v>
+      </c>
+      <c r="G5">
+        <v>2400</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>892500</v>
+      </c>
+      <c r="E6">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F6">
+        <v>2056320000</v>
+      </c>
+      <c r="G6">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2500</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>892500</v>
+      </c>
+      <c r="E7">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F7">
+        <v>2056320000</v>
+      </c>
+      <c r="G7">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2500</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>892500</v>
+      </c>
+      <c r="E8">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F8">
+        <v>2056320000</v>
+      </c>
+      <c r="G8">
+        <v>2400</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2500</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>892500</v>
+      </c>
+      <c r="E9">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F9">
+        <v>2056320000</v>
+      </c>
+      <c r="G9">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2500</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>892500</v>
+      </c>
+      <c r="E10">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F10">
+        <v>2056320000</v>
+      </c>
+      <c r="G10">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2500</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>892500</v>
+      </c>
+      <c r="E11">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F11">
+        <v>2056320000</v>
+      </c>
+      <c r="G11">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2500</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>892500</v>
+      </c>
+      <c r="E12">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F12">
+        <v>2056320000</v>
+      </c>
+      <c r="G12">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2500</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>892500</v>
+      </c>
+      <c r="E13">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F13">
+        <v>2056320000</v>
+      </c>
+      <c r="G13">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2500</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>892500</v>
+      </c>
+      <c r="E14">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F14">
+        <v>2056320000</v>
+      </c>
+      <c r="G14">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2500</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>892500</v>
+      </c>
+      <c r="E15">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F15">
+        <v>2056320000</v>
+      </c>
+      <c r="G15">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2500</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>892500</v>
+      </c>
+      <c r="E16">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F16">
+        <v>2056320000</v>
+      </c>
+      <c r="G16">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2500</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>892500</v>
+      </c>
+      <c r="E17">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F17">
+        <v>2056320000</v>
+      </c>
+      <c r="G17">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2500</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>892500</v>
+      </c>
+      <c r="E18">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F18">
+        <v>2056320000</v>
+      </c>
+      <c r="G18">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2500</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <v>892500</v>
+      </c>
+      <c r="E19">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F19">
+        <v>2056320000</v>
+      </c>
+      <c r="G19">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2500</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="D20">
+        <v>892500</v>
+      </c>
+      <c r="E20">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F20">
+        <v>2056320000</v>
+      </c>
+      <c r="G20">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2500</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>892500</v>
+      </c>
+      <c r="E21">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F21">
+        <v>2056320000</v>
+      </c>
+      <c r="G21">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2500</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>892500</v>
+      </c>
+      <c r="E22">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F22">
+        <v>2056320000</v>
+      </c>
+      <c r="G22">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2500</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>892500</v>
+      </c>
+      <c r="E23">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F23">
+        <v>2056320000</v>
+      </c>
+      <c r="G23">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2500</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>892500</v>
+      </c>
+      <c r="E24">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F24">
+        <v>2056320000</v>
+      </c>
+      <c r="G24">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2500</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25">
+        <v>892500</v>
+      </c>
+      <c r="E25">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F25">
+        <v>2056320000</v>
+      </c>
+      <c r="G25">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2500</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26">
+        <v>892500</v>
+      </c>
+      <c r="E26">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F26">
+        <v>2056320000</v>
+      </c>
+      <c r="G26">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2500</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>892500</v>
+      </c>
+      <c r="E27">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F27">
+        <v>2056320000</v>
+      </c>
+      <c r="G27">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>2500</v>
+      </c>
+      <c r="C28">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>892500</v>
+      </c>
+      <c r="E28">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="F28">
+        <v>2056320000</v>
+      </c>
+      <c r="G28">
+        <v>2400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
@@ -1880,7 +3907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026E4EEC-6CC6-6348-84B2-EA3FB1DE8836}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2539,7 +4566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E704B58D-6420-1E42-86AD-D07BE8D3A93C}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3198,7 +5225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC675B-C02A-EA44-970E-7C58E476B8DE}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3857,7 +5884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF6E03A-F98C-914A-BDEA-46D84952CD42}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -4516,7 +6543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C67EE-3E6E-F147-B360-22D732872280}">
   <dimension ref="A1:G28"/>
   <sheetViews>

</xml_diff>